<commit_message>
[rps update] more progress.
</commit_message>
<xml_diff>
--- a/rps_update/CA_rps.xlsx
+++ b/rps_update/CA_rps.xlsx
@@ -1,41 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paty/wecc_data_migration/rps_update/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="36600" yWindow="400" windowWidth="14180" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -58,13 +65,85 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="37">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -120,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -155,7 +234,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -332,7 +411,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -343,12 +422,12 @@
   <dimension ref="A3:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="B3">
         <v>2020</v>
       </c>
@@ -356,7 +435,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <f>(0.5-0.33)/10</f>
         <v>1.6999999999999998E-2</v>
@@ -369,7 +448,7 @@
         <v>0.34700000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="B5">
         <f>B4+1</f>
         <v>2022</v>
@@ -379,9 +458,9 @@
         <v>0.36400000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="B6">
-        <f t="shared" ref="B6:B16" si="1">B5+1</f>
+        <f t="shared" ref="B6:B13" si="1">B5+1</f>
         <v>2023</v>
       </c>
       <c r="C6">
@@ -389,7 +468,7 @@
         <v>0.38100000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="B7">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -399,7 +478,7 @@
         <v>0.39800000000000008</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="B8">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -409,7 +488,7 @@
         <v>0.41500000000000009</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="B9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -419,7 +498,7 @@
         <v>0.43200000000000011</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="B10">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -429,7 +508,7 @@
         <v>0.44900000000000012</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="B11">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -439,7 +518,7 @@
         <v>0.46600000000000014</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="B12">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -449,7 +528,7 @@
         <v>0.48300000000000015</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="B13">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -461,5 +540,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>